<commit_message>
Edit vacation report excel.
</commit_message>
<xml_diff>
--- a/server/webportal/src/main/resources/template/vacation_template.xlsx
+++ b/server/webportal/src/main/resources/template/vacation_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Kolaer-systems\server\webportal\src\main\resources\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Kolaer-systems\server\webportal\src\main\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Приложение 2.6. Шаблон документа к процессу «2.3.1а. Подготовка графика отпусков»</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>должность сотрудника службы управления персоналом</t>
+  </si>
+  <si>
+    <t>Колатомэнергоремонт - филиал АО "Атомэнергоремонт"</t>
   </si>
 </sst>
 </file>
@@ -329,6 +332,33 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -342,9 +372,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -361,30 +388,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -699,7 +702,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,35 +718,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="29" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="29"/>
+      <c r="H1" s="37"/>
     </row>
     <row r="2" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
+      <c r="A2" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -755,10 +760,10 @@
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="39"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
     </row>
@@ -767,53 +772,53 @@
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
     </row>
     <row r="6" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
     </row>
     <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36" t="s">
+      <c r="F8" s="43"/>
+      <c r="G8" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="36"/>
+      <c r="H8" s="43"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -821,18 +826,18 @@
       <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="38" t="s">
+      <c r="F10" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
@@ -863,10 +868,10 @@
     <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="39" t="s">
+      <c r="C13" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="39"/>
+      <c r="D13" s="32"/>
       <c r="E13" s="10"/>
       <c r="F13" s="11"/>
       <c r="G13" s="12"/>
@@ -883,42 +888,42 @@
       <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40" t="s">
+      <c r="F15" s="33"/>
+      <c r="G15" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="40" t="s">
+      <c r="H15" s="33" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="41"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="34"/>
       <c r="E16" s="14" t="s">
         <v>21</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
@@ -967,56 +972,56 @@
       <c r="H19" s="19"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="21"/>
       <c r="E20" s="22"/>
       <c r="F20" s="23"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
     </row>
     <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="24"/>
       <c r="E21" s="25" t="s">
         <v>24</v>
       </c>
       <c r="F21" s="3"/>
-      <c r="G21" s="31" t="s">
+      <c r="G21" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="H21" s="31"/>
+      <c r="H21" s="28"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="43"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="21"/>
       <c r="E22" s="22"/>
       <c r="F22" s="23"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="42" t="s">
+      <c r="A23" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
       <c r="D23" s="24"/>
       <c r="E23" s="25" t="s">
         <v>24</v>
       </c>
       <c r="F23" s="3"/>
-      <c r="G23" s="31" t="s">
+      <c r="G23" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="31"/>
+      <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
@@ -1024,24 +1029,6 @@
   </sheetData>
   <sheetProtection insertRows="0" deleteRows="0"/>
   <mergeCells count="30">
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:H2"/>
@@ -1054,6 +1041,24 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="G22:H22"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Ошибка!" error="Введите дату в формате дд.мм.гггг." sqref="G13">

</xml_diff>